<commit_message>
fixed errors and started hash lists
</commit_message>
<xml_diff>
--- a/2500 - DiPofi, Dominic.xlsx
+++ b/2500 - DiPofi, Dominic.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0c0653e9e8991524/Documents/Classes/LinDataSTRC/Projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="136" documentId="8_{6788D257-99E1-4CEA-91B2-7F6D15E693B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1CF93041-8AEA-44E3-BC27-DF20CF2A5F80}"/>
+  <xr:revisionPtr revIDLastSave="193" documentId="8_{6788D257-99E1-4CEA-91B2-7F6D15E693B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CA4A930E-34AC-435C-BFE6-37AFFD121710}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{612F62F2-CF27-45EF-9BA4-CBB133109090}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{612F62F2-CF27-45EF-9BA4-CBB133109090}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Run Time for 4 Lists (H, B, W)" sheetId="2" r:id="rId2"/>
+    <sheet name="Run Time for 6 Lists (H, B, W)" sheetId="2" r:id="rId2"/>
     <sheet name="Run Time vs Vocab for List 1" sheetId="3" r:id="rId3"/>
     <sheet name="Run Time vs Key Comp for Hamlet" sheetId="4" r:id="rId4"/>
   </sheets>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
   <si>
     <t>Key Comp</t>
   </si>
@@ -115,6 +115,33 @@
   </si>
   <si>
     <t>4W</t>
+  </si>
+  <si>
+    <t>2aH</t>
+  </si>
+  <si>
+    <t>2aB</t>
+  </si>
+  <si>
+    <t>2aW</t>
+  </si>
+  <si>
+    <t>5H</t>
+  </si>
+  <si>
+    <t>5W</t>
+  </si>
+  <si>
+    <t>5B</t>
+  </si>
+  <si>
+    <t>Sorted Modified</t>
+  </si>
+  <si>
+    <t>Skip List</t>
+  </si>
+  <si>
+    <t>h</t>
   </si>
 </sst>
 </file>
@@ -223,7 +250,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Time for 4 Lists for Hamlet, Bleak House, War and Peace</a:t>
+              <a:t> Time for 6 Lists for Hamlet, Bleak House, War and Peace</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -280,9 +307,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Data!$B$3:$B$14</c:f>
+              <c:f>Data!$B$3:$B$20</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>1H</c:v>
                 </c:pt>
@@ -290,44 +317,62 @@
                   <c:v>2H</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>2aH</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>3H</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>4H</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>5H</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>1B</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>2B</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
+                  <c:v>2aB</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>3B</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>4B</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
+                  <c:v>5B</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>1W</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="13">
                   <c:v>2W</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="14">
+                  <c:v>2aW</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>3W</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="16">
                   <c:v>4W</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5W</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$D$3:$D$14</c:f>
+              <c:f>Data!$D$3:$D$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>1.0349999999999999</c:v>
                 </c:pt>
@@ -335,34 +380,52 @@
                   <c:v>0.42899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.432</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.254</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>1.0229999999999999</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>3.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>36.743000000000002</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>25.262</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
+                  <c:v>20.245000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>5.8819999999999997</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>39.963000000000001</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
+                  <c:v>0.111</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>48.643000000000001</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="13">
                   <c:v>38.359000000000002</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="14">
+                  <c:v>27.271000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>8.7080000000000002</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="16">
                   <c:v>54.13</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -755,7 +818,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>(Data!$D$3,Data!$D$7,Data!$D$11)</c:f>
+              <c:f>(Data!$D$3,Data!$D$9,Data!$D$15)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -773,7 +836,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(Data!$E$3,Data!$E$7,Data!$E$11)</c:f>
+              <c:f>(Data!$E$3,Data!$E$9,Data!$E$15)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1206,10 +1269,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>(Data!$D$3,Data!$D$4,Data!$D$5,Data!$D$6)</c:f>
+              <c:f>(Data!$D$3,Data!$D$4,Data!$D$5,Data!$D$6,Data!$D$7,Data!$D$8)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1.0349999999999999</c:v>
                 </c:pt>
@@ -1217,20 +1280,26 @@
                   <c:v>0.42899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.432</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.254</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>1.0229999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(Data!$G$3,Data!$G$4,Data!$G$5,Data!$G$6)</c:f>
+              <c:f>(Data!$G$3,Data!$G$4,Data!$G$5,Data!$G$6,Data!$G$7,Data!$G$8)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>80116080</c:v>
                 </c:pt>
@@ -1238,10 +1307,16 @@
                   <c:v>48831609</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>32730336</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>20511561</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>77134244</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>635042</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3206,7 +3281,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{584CFFAD-DE03-4D83-B784-450007249840}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3631,10 +3706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF66162F-62E8-4BFF-849A-72621D5831F7}">
-  <dimension ref="A2:H19"/>
+  <dimension ref="A2:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3643,7 +3718,7 @@
     <col min="3" max="8" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -3665,8 +3740,11 @@
       <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="I2" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -3692,7 +3770,7 @@
         <v>9608</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>15</v>
       </c>
@@ -3715,15 +3793,15 @@
         <v>9608</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="D5">
-        <v>0.254</v>
+        <v>0.432</v>
       </c>
       <c r="E5">
         <v>4804</v>
@@ -3732,21 +3810,21 @@
         <v>31991</v>
       </c>
       <c r="G5">
-        <v>20511561</v>
+        <v>32730336</v>
       </c>
       <c r="H5">
-        <v>90800</v>
+        <v>9608</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6">
-        <v>1.0229999999999999</v>
+        <v>0.254</v>
       </c>
       <c r="E6">
         <v>4804</v>
@@ -3755,70 +3833,73 @@
         <v>31991</v>
       </c>
       <c r="G6">
+        <v>20511561</v>
+      </c>
+      <c r="H6">
+        <v>90800</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>1.0229999999999999</v>
+      </c>
+      <c r="E7">
+        <v>4804</v>
+      </c>
+      <c r="F7">
+        <v>31991</v>
+      </c>
+      <c r="G7">
         <v>77134244</v>
       </c>
-      <c r="H6">
+      <c r="H7">
         <v>90965</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E8">
+        <v>4804</v>
+      </c>
+      <c r="F8">
+        <v>31991</v>
+      </c>
+      <c r="G8">
+        <v>635042</v>
+      </c>
+      <c r="H8">
+        <v>57102</v>
+      </c>
+      <c r="I8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C9" t="s">
         <v>7</v>
       </c>
-      <c r="D7">
+      <c r="D9">
         <v>36.743000000000002</v>
-      </c>
-      <c r="E7">
-        <v>17947</v>
-      </c>
-      <c r="F7">
-        <v>353461</v>
-      </c>
-      <c r="G7">
-        <v>3864805384</v>
-      </c>
-      <c r="H7">
-        <v>35882</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8">
-        <v>25.262</v>
-      </c>
-      <c r="E8">
-        <v>17947</v>
-      </c>
-      <c r="F8">
-        <v>353461</v>
-      </c>
-      <c r="G8">
-        <v>2271614447</v>
-      </c>
-      <c r="H8">
-        <v>35882</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9">
-        <v>5.8819999999999997</v>
       </c>
       <c r="E9">
         <v>17947</v>
@@ -3827,21 +3908,21 @@
         <v>353461</v>
       </c>
       <c r="G9">
-        <v>428180670</v>
+        <v>3864805384</v>
       </c>
       <c r="H9">
-        <v>1040960</v>
+        <v>35882</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D10">
-        <v>39.963000000000001</v>
+        <v>25.262</v>
       </c>
       <c r="E10">
         <v>17947</v>
@@ -3850,119 +3931,263 @@
         <v>353461</v>
       </c>
       <c r="G10">
+        <v>2271614447</v>
+      </c>
+      <c r="H10">
+        <v>35882</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11">
+        <v>20.245000000000001</v>
+      </c>
+      <c r="E11">
+        <v>17947</v>
+      </c>
+      <c r="F11">
+        <v>353461</v>
+      </c>
+      <c r="G11">
+        <v>1544987797</v>
+      </c>
+      <c r="H11">
+        <v>35882</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12">
+        <v>5.8819999999999997</v>
+      </c>
+      <c r="E12">
+        <v>17947</v>
+      </c>
+      <c r="F12">
+        <v>353461</v>
+      </c>
+      <c r="G12">
+        <v>428180670</v>
+      </c>
+      <c r="H12">
+        <v>1040960</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>39.963000000000001</v>
+      </c>
+      <c r="E13">
+        <v>17947</v>
+      </c>
+      <c r="F13">
+        <v>353461</v>
+      </c>
+      <c r="G13">
         <v>3364682624</v>
       </c>
-      <c r="H10">
+      <c r="H13">
         <v>1041548</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14">
+        <v>0.111</v>
+      </c>
+      <c r="E14">
+        <v>17947</v>
+      </c>
+      <c r="F14">
+        <v>353461</v>
+      </c>
+      <c r="G14">
+        <v>8609758</v>
+      </c>
+      <c r="H14">
+        <v>216101</v>
+      </c>
+      <c r="I14">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B15" t="s">
         <v>22</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C15" t="s">
         <v>7</v>
       </c>
-      <c r="D11">
+      <c r="D15">
         <v>48.643000000000001</v>
       </c>
-      <c r="E11">
+      <c r="E15">
         <v>20327</v>
       </c>
-      <c r="F11">
+      <c r="F15">
         <v>563023</v>
       </c>
-      <c r="G11">
+      <c r="G15">
         <v>6738758767</v>
       </c>
-      <c r="H11">
+      <c r="H15">
         <v>40470</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>23</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C16" t="s">
         <v>8</v>
       </c>
-      <c r="D12">
+      <c r="D16">
         <v>38.359000000000002</v>
       </c>
-      <c r="E12">
+      <c r="E16">
         <v>20327</v>
       </c>
-      <c r="F12">
+      <c r="F16">
         <v>563023</v>
       </c>
-      <c r="G12">
+      <c r="G16">
         <v>3982656802</v>
       </c>
-      <c r="H12">
+      <c r="H16">
         <v>40470</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17">
+        <v>27.271000000000001</v>
+      </c>
+      <c r="E17">
+        <v>20327</v>
+      </c>
+      <c r="F17">
+        <v>563023</v>
+      </c>
+      <c r="G17">
+        <v>2747648070</v>
+      </c>
+      <c r="H17">
+        <v>40470</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>24</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C18" t="s">
         <v>9</v>
       </c>
-      <c r="D13">
+      <c r="D18">
         <v>8.7080000000000002</v>
       </c>
-      <c r="E13">
+      <c r="E18">
         <v>20327</v>
       </c>
-      <c r="F13">
+      <c r="F18">
         <v>563023</v>
       </c>
-      <c r="G13">
+      <c r="G18">
         <v>654493106</v>
       </c>
-      <c r="H13">
+      <c r="H18">
         <v>1665945</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>25</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C19" t="s">
         <v>10</v>
       </c>
-      <c r="D14">
+      <c r="D19">
         <v>54.13</v>
       </c>
-      <c r="E14">
+      <c r="E19">
         <v>20327</v>
       </c>
-      <c r="F14">
+      <c r="F19">
         <v>563023</v>
       </c>
-      <c r="G14">
+      <c r="G19">
         <v>5378251682</v>
       </c>
-      <c r="H14">
+      <c r="H19">
         <v>1624746</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20">
+        <v>0.17</v>
+      </c>
+      <c r="E20">
+        <v>20327</v>
+      </c>
+      <c r="F20">
+        <v>563023</v>
+      </c>
+      <c r="G20">
+        <v>15369920</v>
+      </c>
+      <c r="H20">
+        <v>243253</v>
+      </c>
+      <c r="I20">
+        <v>24</v>
+      </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>